<commit_message>
stuff associating clincial trials with resistance in vivo results.
</commit_message>
<xml_diff>
--- a/tabular/contributed/180326 SOF VEL TABLE.xlsx
+++ b/tabular/contributed/180326 SOF VEL TABLE.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13100" yWindow="5480" windowWidth="34240" windowHeight="20960"/>
+    <workbookView xWindow="15320" yWindow="7120" windowWidth="34240" windowHeight="18000" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="VEL" sheetId="1" r:id="rId1"/>
@@ -59,9 +59,6 @@
   </si>
   <si>
     <t>30E</t>
-  </si>
-  <si>
-    <t>EASL 2013 Poster 1191</t>
   </si>
   <si>
     <t>30R</t>
@@ -684,6 +681,9 @@
   </si>
   <si>
     <t>pubmed</t>
+  </si>
+  <si>
+    <t>EASL_2013_Poster_1191</t>
   </si>
 </sst>
 </file>
@@ -1200,8 +1200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="E1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B1" sqref="B1:L123"/>
     </sheetView>
   </sheetViews>
@@ -1226,34 +1226,34 @@
         <v>4</v>
       </c>
       <c r="B1" s="30" t="s">
+        <v>157</v>
+      </c>
+      <c r="C1" s="20" t="s">
         <v>158</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="D1" s="20" t="s">
         <v>159</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="E1" s="30" t="s">
         <v>160</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="F1" s="21" t="s">
         <v>161</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="G1" s="30" t="s">
         <v>162</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="H1" s="30" t="s">
         <v>163</v>
       </c>
-      <c r="H1" s="30" t="s">
+      <c r="I1" s="31" t="s">
         <v>164</v>
       </c>
-      <c r="I1" s="31" t="s">
+      <c r="J1" s="22" t="s">
         <v>165</v>
       </c>
-      <c r="J1" s="22" t="s">
+      <c r="K1" s="23" t="s">
         <v>166</v>
-      </c>
-      <c r="K1" s="23" t="s">
-        <v>167</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>3</v>
@@ -1268,7 +1268,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D2" s="20" t="s">
         <v>8</v>
@@ -1277,14 +1277,14 @@
         <v>2</v>
       </c>
       <c r="F2" s="21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G2" s="20"/>
       <c r="H2" s="20"/>
       <c r="I2" s="20"/>
       <c r="J2" s="20"/>
       <c r="K2" s="23" t="s">
-        <v>10</v>
+        <v>167</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="1"/>
@@ -1313,7 +1313,7 @@
       <c r="I3" s="20"/>
       <c r="J3" s="20"/>
       <c r="K3" s="23" t="s">
-        <v>10</v>
+        <v>167</v>
       </c>
       <c r="L3" s="2"/>
       <c r="M3" s="1"/>
@@ -1342,7 +1342,7 @@
       <c r="I4" s="20"/>
       <c r="J4" s="20"/>
       <c r="K4" s="23" t="s">
-        <v>10</v>
+        <v>167</v>
       </c>
       <c r="L4" s="2"/>
       <c r="M4" s="1"/>
@@ -1355,7 +1355,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" s="20" t="s">
         <v>8</v>
@@ -1371,7 +1371,7 @@
       <c r="I5" s="20"/>
       <c r="J5" s="20"/>
       <c r="K5" s="23" t="s">
-        <v>10</v>
+        <v>167</v>
       </c>
       <c r="L5" s="2"/>
       <c r="M5" s="1"/>
@@ -1384,7 +1384,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D6" s="20" t="s">
         <v>8</v>
@@ -1393,14 +1393,14 @@
         <v>2</v>
       </c>
       <c r="F6" s="21" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G6" s="20"/>
       <c r="H6" s="20"/>
       <c r="I6" s="20"/>
       <c r="J6" s="20"/>
       <c r="K6" s="23" t="s">
-        <v>10</v>
+        <v>167</v>
       </c>
       <c r="L6" s="2"/>
       <c r="M6" s="1"/>
@@ -1413,7 +1413,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D7" s="20" t="s">
         <v>8</v>
@@ -1429,7 +1429,7 @@
       <c r="I7" s="20"/>
       <c r="J7" s="20"/>
       <c r="K7" s="23" t="s">
-        <v>10</v>
+        <v>167</v>
       </c>
       <c r="L7" s="2"/>
       <c r="M7" s="1"/>
@@ -1439,10 +1439,10 @@
         <v>5</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D8" s="20" t="s">
         <v>8</v>
@@ -1451,14 +1451,14 @@
         <v>2</v>
       </c>
       <c r="F8" s="21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G8" s="20"/>
       <c r="H8" s="20"/>
       <c r="I8" s="20"/>
       <c r="J8" s="20"/>
       <c r="K8" s="23" t="s">
-        <v>10</v>
+        <v>167</v>
       </c>
       <c r="L8" s="2"/>
       <c r="M8" s="1"/>
@@ -1468,10 +1468,10 @@
         <v>5</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D9" s="20" t="s">
         <v>8</v>
@@ -1480,14 +1480,14 @@
         <v>2</v>
       </c>
       <c r="F9" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G9" s="20"/>
       <c r="H9" s="20"/>
       <c r="I9" s="20"/>
       <c r="J9" s="20"/>
       <c r="K9" s="23" t="s">
-        <v>10</v>
+        <v>167</v>
       </c>
       <c r="L9" s="2"/>
       <c r="M9" s="1"/>
@@ -1497,10 +1497,10 @@
         <v>5</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D10" s="20" t="s">
         <v>8</v>
@@ -1516,7 +1516,7 @@
       <c r="I10" s="20"/>
       <c r="J10" s="20"/>
       <c r="K10" s="23" t="s">
-        <v>10</v>
+        <v>167</v>
       </c>
       <c r="L10" s="2"/>
       <c r="M10" s="1"/>
@@ -1526,7 +1526,7 @@
         <v>5</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" s="20" t="s">
         <v>7</v>
@@ -1545,7 +1545,7 @@
       <c r="I11" s="20"/>
       <c r="J11" s="20"/>
       <c r="K11" s="23" t="s">
-        <v>10</v>
+        <v>167</v>
       </c>
       <c r="L11" s="3"/>
       <c r="M11" s="1"/>
@@ -1558,7 +1558,7 @@
         <v>1</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D12" s="20" t="s">
         <v>8</v>
@@ -1567,7 +1567,7 @@
         <v>2</v>
       </c>
       <c r="F12" s="21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G12" s="20"/>
       <c r="H12" s="20"/>
@@ -1587,7 +1587,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D13" s="20" t="s">
         <v>8</v>
@@ -1596,7 +1596,7 @@
         <v>2</v>
       </c>
       <c r="F13" s="21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G13" s="20"/>
       <c r="H13" s="20"/>
@@ -1625,7 +1625,7 @@
         <v>2</v>
       </c>
       <c r="F14" s="21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G14" s="20"/>
       <c r="H14" s="20"/>
@@ -1645,16 +1645,16 @@
         <v>1</v>
       </c>
       <c r="C15" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" s="25" t="s">
         <v>15</v>
-      </c>
-      <c r="D15" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="F15" s="25" t="s">
-        <v>16</v>
       </c>
       <c r="G15" s="20"/>
       <c r="H15" s="20"/>
@@ -1674,7 +1674,7 @@
         <v>1</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D16" s="20" t="s">
         <v>8</v>
@@ -1683,7 +1683,7 @@
         <v>2</v>
       </c>
       <c r="F16" s="21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G16" s="20"/>
       <c r="H16" s="20"/>
@@ -1703,7 +1703,7 @@
         <v>1</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D17" s="20" t="s">
         <v>8</v>
@@ -1712,7 +1712,7 @@
         <v>2</v>
       </c>
       <c r="F17" s="21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G17" s="20"/>
       <c r="H17" s="20"/>
@@ -1729,19 +1729,19 @@
         <v>5</v>
       </c>
       <c r="B18" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" s="21" t="s">
         <v>19</v>
-      </c>
-      <c r="C18" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="F18" s="21" t="s">
-        <v>20</v>
       </c>
       <c r="G18" s="20"/>
       <c r="H18" s="20"/>
@@ -1758,10 +1758,10 @@
         <v>5</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D19" s="20" t="s">
         <v>8</v>
@@ -1770,7 +1770,7 @@
         <v>2</v>
       </c>
       <c r="F19" s="21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G19" s="20"/>
       <c r="H19" s="20"/>
@@ -1787,10 +1787,10 @@
         <v>5</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D20" s="20" t="s">
         <v>8</v>
@@ -1799,7 +1799,7 @@
         <v>2</v>
       </c>
       <c r="F20" s="21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G20" s="20"/>
       <c r="H20" s="20"/>
@@ -1816,10 +1816,10 @@
         <v>5</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D21" s="20" t="s">
         <v>8</v>
@@ -1828,7 +1828,7 @@
         <v>2</v>
       </c>
       <c r="F21" s="21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G21" s="20"/>
       <c r="H21" s="20"/>
@@ -1843,7 +1843,7 @@
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="10"/>
       <c r="B22" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C22" s="20" t="s">
         <v>7</v>
@@ -1855,7 +1855,7 @@
         <v>2</v>
       </c>
       <c r="F22" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G22" s="20"/>
       <c r="H22" s="20"/>
@@ -1872,7 +1872,7 @@
         <v>5</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C23" s="20" t="s">
         <v>7</v>
@@ -1884,7 +1884,7 @@
         <v>2</v>
       </c>
       <c r="F23" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G23" s="20"/>
       <c r="H23" s="20"/>
@@ -1901,11 +1901,11 @@
         <v>5</v>
       </c>
       <c r="B24" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="20" t="s">
-        <v>22</v>
-      </c>
       <c r="D24" s="20" t="s">
         <v>8</v>
       </c>
@@ -1913,7 +1913,7 @@
         <v>2</v>
       </c>
       <c r="F24" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G24" s="20"/>
       <c r="H24" s="20"/>
@@ -1930,10 +1930,10 @@
         <v>5</v>
       </c>
       <c r="B25" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D25" s="20" t="s">
         <v>8</v>
@@ -1942,7 +1942,7 @@
         <v>2</v>
       </c>
       <c r="F25" s="25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G25" s="20"/>
       <c r="H25" s="20"/>
@@ -1959,10 +1959,10 @@
         <v>5</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D26" s="20" t="s">
         <v>8</v>
@@ -1971,7 +1971,7 @@
         <v>2</v>
       </c>
       <c r="F26" s="25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G26" s="20"/>
       <c r="H26" s="20"/>
@@ -1988,10 +1988,10 @@
         <v>5</v>
       </c>
       <c r="B27" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D27" s="20" t="s">
         <v>8</v>
@@ -2000,7 +2000,7 @@
         <v>2</v>
       </c>
       <c r="F27" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G27" s="20"/>
       <c r="H27" s="20"/>
@@ -2017,10 +2017,10 @@
         <v>5</v>
       </c>
       <c r="B28" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D28" s="20" t="s">
         <v>8</v>
@@ -2029,7 +2029,7 @@
         <v>2</v>
       </c>
       <c r="F28" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G28" s="20"/>
       <c r="H28" s="20"/>
@@ -2046,11 +2046,11 @@
         <v>5</v>
       </c>
       <c r="B29" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="C29" s="20" t="s">
-        <v>35</v>
-      </c>
       <c r="D29" s="20" t="s">
         <v>8</v>
       </c>
@@ -2058,7 +2058,7 @@
         <v>2</v>
       </c>
       <c r="F29" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G29" s="20"/>
       <c r="H29" s="20"/>
@@ -2075,10 +2075,10 @@
         <v>5</v>
       </c>
       <c r="B30" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D30" s="20" t="s">
         <v>8</v>
@@ -2087,7 +2087,7 @@
         <v>2</v>
       </c>
       <c r="F30" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G30" s="20"/>
       <c r="H30" s="20"/>
@@ -2104,10 +2104,10 @@
         <v>5</v>
       </c>
       <c r="B31" s="20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D31" s="20" t="s">
         <v>8</v>
@@ -2116,7 +2116,7 @@
         <v>2</v>
       </c>
       <c r="F31" s="25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G31" s="20"/>
       <c r="H31" s="20"/>
@@ -2133,10 +2133,10 @@
         <v>5</v>
       </c>
       <c r="B32" s="20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D32" s="20" t="s">
         <v>8</v>
@@ -2145,7 +2145,7 @@
         <v>2</v>
       </c>
       <c r="F32" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G32" s="20"/>
       <c r="H32" s="20"/>
@@ -2162,7 +2162,7 @@
         <v>5</v>
       </c>
       <c r="B33" s="20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C33" s="20" t="s">
         <v>7</v>
@@ -2174,7 +2174,7 @@
         <v>2</v>
       </c>
       <c r="F33" s="25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G33" s="20"/>
       <c r="H33" s="20"/>
@@ -2191,10 +2191,10 @@
         <v>5</v>
       </c>
       <c r="B34" s="20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C34" s="20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D34" s="20" t="s">
         <v>8</v>
@@ -2203,7 +2203,7 @@
         <v>2</v>
       </c>
       <c r="F34" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G34" s="20"/>
       <c r="H34" s="20"/>
@@ -2220,19 +2220,19 @@
         <v>5</v>
       </c>
       <c r="B35" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="D35" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="F35" s="25" t="s">
         <v>13</v>
-      </c>
-      <c r="C35" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="D35" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="E35" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="F35" s="25" t="s">
-        <v>14</v>
       </c>
       <c r="G35" s="20"/>
       <c r="H35" s="20"/>
@@ -2249,10 +2249,10 @@
         <v>5</v>
       </c>
       <c r="B36" s="20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C36" s="20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D36" s="20" t="s">
         <v>8</v>
@@ -2261,7 +2261,7 @@
         <v>2</v>
       </c>
       <c r="F36" s="25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G36" s="20"/>
       <c r="H36" s="20"/>
@@ -2278,10 +2278,10 @@
         <v>5</v>
       </c>
       <c r="B37" s="20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C37" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D37" s="20" t="s">
         <v>8</v>
@@ -2290,7 +2290,7 @@
         <v>2</v>
       </c>
       <c r="F37" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G37" s="20"/>
       <c r="H37" s="20"/>
@@ -2307,10 +2307,10 @@
         <v>5</v>
       </c>
       <c r="B38" s="20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C38" s="20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D38" s="20" t="s">
         <v>8</v>
@@ -2319,7 +2319,7 @@
         <v>2</v>
       </c>
       <c r="F38" s="25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G38" s="20"/>
       <c r="H38" s="20"/>
@@ -2339,16 +2339,16 @@
         <v>1</v>
       </c>
       <c r="C39" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D39" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E39" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="F39" s="25" t="s">
         <v>37</v>
-      </c>
-      <c r="D39" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="E39" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="F39" s="25" t="s">
-        <v>38</v>
       </c>
       <c r="G39" s="20"/>
       <c r="H39" s="20"/>
@@ -2377,7 +2377,7 @@
         <v>2</v>
       </c>
       <c r="F40" s="25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G40" s="20"/>
       <c r="H40" s="20"/>
@@ -2397,16 +2397,16 @@
         <v>1</v>
       </c>
       <c r="C41" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="D41" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E41" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="F41" s="25" t="s">
         <v>40</v>
-      </c>
-      <c r="D41" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="E41" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="F41" s="25" t="s">
-        <v>41</v>
       </c>
       <c r="G41" s="20"/>
       <c r="H41" s="20"/>
@@ -2426,7 +2426,7 @@
         <v>1</v>
       </c>
       <c r="C42" s="20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D42" s="20" t="s">
         <v>8</v>
@@ -2435,7 +2435,7 @@
         <v>2</v>
       </c>
       <c r="F42" s="25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G42" s="20"/>
       <c r="H42" s="20"/>
@@ -2455,7 +2455,7 @@
         <v>1</v>
       </c>
       <c r="C43" s="20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D43" s="20" t="s">
         <v>8</v>
@@ -2464,7 +2464,7 @@
         <v>2</v>
       </c>
       <c r="F43" s="25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G43" s="20"/>
       <c r="H43" s="20"/>
@@ -2484,7 +2484,7 @@
         <v>1</v>
       </c>
       <c r="C44" s="24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D44" s="20" t="s">
         <v>8</v>
@@ -2493,7 +2493,7 @@
         <v>2</v>
       </c>
       <c r="F44" s="25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G44" s="24"/>
       <c r="H44" s="24"/>
@@ -2513,7 +2513,7 @@
         <v>1</v>
       </c>
       <c r="C45" s="24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D45" s="20" t="s">
         <v>8</v>
@@ -2522,7 +2522,7 @@
         <v>2</v>
       </c>
       <c r="F45" s="25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G45" s="24"/>
       <c r="H45" s="24"/>
@@ -2542,16 +2542,16 @@
         <v>1</v>
       </c>
       <c r="C46" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="D46" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E46" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="F46" s="25" t="s">
         <v>46</v>
-      </c>
-      <c r="D46" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="E46" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="F46" s="25" t="s">
-        <v>47</v>
       </c>
       <c r="G46" s="24"/>
       <c r="H46" s="24"/>
@@ -2571,16 +2571,16 @@
         <v>1</v>
       </c>
       <c r="C47" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="D47" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E47" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="F47" s="25" t="s">
         <v>48</v>
-      </c>
-      <c r="D47" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="E47" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="F47" s="25" t="s">
-        <v>49</v>
       </c>
       <c r="G47" s="24"/>
       <c r="H47" s="24"/>
@@ -2600,16 +2600,16 @@
         <v>1</v>
       </c>
       <c r="C48" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="D48" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E48" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="F48" s="25" t="s">
         <v>50</v>
-      </c>
-      <c r="D48" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="E48" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="F48" s="25" t="s">
-        <v>51</v>
       </c>
       <c r="G48" s="24"/>
       <c r="H48" s="24"/>
@@ -2629,7 +2629,7 @@
         <v>1</v>
       </c>
       <c r="C49" s="24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D49" s="20" t="s">
         <v>8</v>
@@ -2638,7 +2638,7 @@
         <v>2</v>
       </c>
       <c r="F49" s="25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G49" s="24"/>
       <c r="H49" s="24"/>
@@ -2667,7 +2667,7 @@
         <v>2</v>
       </c>
       <c r="F50" s="25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G50" s="24"/>
       <c r="H50" s="24"/>
@@ -2687,7 +2687,7 @@
         <v>1</v>
       </c>
       <c r="C51" s="24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D51" s="20" t="s">
         <v>8</v>
@@ -2696,7 +2696,7 @@
         <v>2</v>
       </c>
       <c r="F51" s="25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G51" s="24"/>
       <c r="H51" s="24"/>
@@ -2716,16 +2716,16 @@
         <v>1</v>
       </c>
       <c r="C52" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="D52" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E52" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="F52" s="25" t="s">
         <v>55</v>
-      </c>
-      <c r="D52" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="E52" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="F52" s="25" t="s">
-        <v>56</v>
       </c>
       <c r="G52" s="24"/>
       <c r="H52" s="24"/>
@@ -2745,16 +2745,16 @@
         <v>1</v>
       </c>
       <c r="C53" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="D53" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E53" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="F53" s="25" t="s">
         <v>57</v>
-      </c>
-      <c r="D53" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="E53" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="F53" s="25" t="s">
-        <v>58</v>
       </c>
       <c r="G53" s="24"/>
       <c r="H53" s="24"/>
@@ -2774,16 +2774,16 @@
         <v>1</v>
       </c>
       <c r="C54" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="D54" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E54" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="F54" s="25" t="s">
         <v>59</v>
-      </c>
-      <c r="D54" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="E54" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="F54" s="25" t="s">
-        <v>60</v>
       </c>
       <c r="G54" s="24"/>
       <c r="H54" s="24"/>
@@ -2803,16 +2803,16 @@
         <v>1</v>
       </c>
       <c r="C55" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="D55" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E55" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="F55" s="25" t="s">
         <v>61</v>
-      </c>
-      <c r="D55" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="E55" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="F55" s="25" t="s">
-        <v>62</v>
       </c>
       <c r="G55" s="24"/>
       <c r="H55" s="24"/>
@@ -2832,16 +2832,16 @@
         <v>1</v>
       </c>
       <c r="C56" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="D56" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E56" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="F56" s="25" t="s">
         <v>63</v>
-      </c>
-      <c r="D56" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="E56" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="F56" s="25" t="s">
-        <v>64</v>
       </c>
       <c r="G56" s="24"/>
       <c r="H56" s="24"/>
@@ -2861,16 +2861,16 @@
         <v>1</v>
       </c>
       <c r="C57" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="D57" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E57" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="F57" s="25" t="s">
         <v>65</v>
-      </c>
-      <c r="D57" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="E57" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="F57" s="25" t="s">
-        <v>66</v>
       </c>
       <c r="G57" s="24"/>
       <c r="H57" s="24"/>
@@ -2890,16 +2890,16 @@
         <v>1</v>
       </c>
       <c r="C58" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="D58" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E58" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="F58" s="25" t="s">
         <v>67</v>
-      </c>
-      <c r="D58" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="E58" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="F58" s="25" t="s">
-        <v>68</v>
       </c>
       <c r="G58" s="24"/>
       <c r="H58" s="24"/>
@@ -2919,16 +2919,16 @@
         <v>1</v>
       </c>
       <c r="C59" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="D59" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E59" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="F59" s="25" t="s">
         <v>69</v>
-      </c>
-      <c r="D59" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="E59" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="F59" s="25" t="s">
-        <v>70</v>
       </c>
       <c r="G59" s="24"/>
       <c r="H59" s="24"/>
@@ -2945,7 +2945,7 @@
         <v>5</v>
       </c>
       <c r="B60" s="24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C60" s="24" t="s">
         <v>7</v>
@@ -2957,7 +2957,7 @@
         <v>2</v>
       </c>
       <c r="F60" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G60" s="24"/>
       <c r="H60" s="24"/>
@@ -2974,10 +2974,10 @@
         <v>5</v>
       </c>
       <c r="B61" s="24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C61" s="24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D61" s="20" t="s">
         <v>8</v>
@@ -2986,7 +2986,7 @@
         <v>2</v>
       </c>
       <c r="F61" s="25" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G61" s="24"/>
       <c r="H61" s="24"/>
@@ -3003,10 +3003,10 @@
         <v>5</v>
       </c>
       <c r="B62" s="24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C62" s="24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D62" s="20" t="s">
         <v>8</v>
@@ -3015,7 +3015,7 @@
         <v>2</v>
       </c>
       <c r="F62" s="25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G62" s="24"/>
       <c r="H62" s="24"/>
@@ -3032,10 +3032,10 @@
         <v>5</v>
       </c>
       <c r="B63" s="24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C63" s="24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D63" s="20" t="s">
         <v>8</v>
@@ -3044,7 +3044,7 @@
         <v>2</v>
       </c>
       <c r="F63" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G63" s="24"/>
       <c r="H63" s="24"/>
@@ -3061,7 +3061,7 @@
         <v>5</v>
       </c>
       <c r="B64" s="24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C64" s="24" t="s">
         <v>7</v>
@@ -3073,7 +3073,7 @@
         <v>2</v>
       </c>
       <c r="F64" s="25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G64" s="24"/>
       <c r="H64" s="24"/>
@@ -3090,7 +3090,7 @@
         <v>5</v>
       </c>
       <c r="B65" s="24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C65" s="24" t="s">
         <v>7</v>
@@ -3102,7 +3102,7 @@
         <v>2</v>
       </c>
       <c r="F65" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G65" s="24"/>
       <c r="H65" s="24"/>
@@ -3119,10 +3119,10 @@
         <v>5</v>
       </c>
       <c r="B66" s="24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C66" s="24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D66" s="20" t="s">
         <v>8</v>
@@ -3131,7 +3131,7 @@
         <v>2</v>
       </c>
       <c r="F66" s="25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G66" s="24"/>
       <c r="H66" s="24"/>
@@ -3148,10 +3148,10 @@
         <v>5</v>
       </c>
       <c r="B67" s="24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C67" s="24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D67" s="20" t="s">
         <v>8</v>
@@ -3160,7 +3160,7 @@
         <v>2</v>
       </c>
       <c r="F67" s="25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G67" s="24"/>
       <c r="H67" s="24"/>
@@ -3177,19 +3177,19 @@
         <v>5</v>
       </c>
       <c r="B68" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="C68" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="D68" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E68" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="F68" s="25" t="s">
         <v>78</v>
-      </c>
-      <c r="C68" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="D68" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="E68" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="F68" s="25" t="s">
-        <v>79</v>
       </c>
       <c r="G68" s="24"/>
       <c r="H68" s="24"/>
@@ -3206,7 +3206,7 @@
         <v>5</v>
       </c>
       <c r="B69" s="24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C69" s="24" t="s">
         <v>7</v>
@@ -3218,7 +3218,7 @@
         <v>2</v>
       </c>
       <c r="F69" s="25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G69" s="24"/>
       <c r="H69" s="24"/>
@@ -3235,10 +3235,10 @@
         <v>5</v>
       </c>
       <c r="B70" s="24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C70" s="24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D70" s="20" t="s">
         <v>8</v>
@@ -3247,7 +3247,7 @@
         <v>2</v>
       </c>
       <c r="F70" s="25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G70" s="24"/>
       <c r="H70" s="24"/>
@@ -3267,26 +3267,26 @@
         <v>1</v>
       </c>
       <c r="C71" s="24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D71" s="20" t="s">
         <v>8</v>
       </c>
       <c r="E71" s="24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F71" s="25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G71" s="24" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H71" s="26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I71" s="24"/>
       <c r="J71" s="24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K71" s="18">
         <v>29221887</v>
@@ -3308,20 +3308,20 @@
         <v>8</v>
       </c>
       <c r="E72" s="24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F72" s="25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G72" s="24" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H72" s="26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I72" s="24"/>
       <c r="J72" s="24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K72" s="18">
         <v>29221887</v>
@@ -3334,29 +3334,29 @@
         <v>5</v>
       </c>
       <c r="B73" s="24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C73" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D73" s="20" t="s">
         <v>8</v>
       </c>
       <c r="E73" s="24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F73" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G73" s="24" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H73" s="26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I73" s="24"/>
       <c r="J73" s="24" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K73" s="18">
         <v>29221887</v>
@@ -3369,10 +3369,10 @@
         <v>5</v>
       </c>
       <c r="B74" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C74" s="24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D74" s="20" t="s">
         <v>8</v>
@@ -3381,17 +3381,17 @@
         <v>0</v>
       </c>
       <c r="F74" s="25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G74" s="24" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H74" s="26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I74" s="24"/>
       <c r="J74" s="24" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K74" s="18">
         <v>29221887</v>
@@ -3404,29 +3404,29 @@
         <v>5</v>
       </c>
       <c r="B75" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C75" s="24" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D75" s="20" t="s">
         <v>8</v>
       </c>
       <c r="E75" s="24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F75" s="25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G75" s="24" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H75" s="26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I75" s="24"/>
       <c r="J75" s="27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K75" s="18">
         <v>29221887</v>
@@ -3439,10 +3439,10 @@
         <v>5</v>
       </c>
       <c r="B76" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C76" s="24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D76" s="29" t="s">
         <v>8</v>
@@ -3451,17 +3451,17 @@
         <v>0</v>
       </c>
       <c r="F76" s="25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G76" s="24" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H76" s="26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I76" s="24"/>
       <c r="J76" s="24" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K76" s="18">
         <v>29221887</v>
@@ -3474,29 +3474,29 @@
         <v>5</v>
       </c>
       <c r="B77" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C77" s="24" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D77" s="29" t="s">
         <v>8</v>
       </c>
       <c r="E77" s="24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F77" s="25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G77" s="24" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H77" s="26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I77" s="24"/>
       <c r="J77" s="27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K77" s="18">
         <v>29221887</v>
@@ -3509,7 +3509,7 @@
         <v>5</v>
       </c>
       <c r="B78" s="24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C78" s="24" t="s">
         <v>7</v>
@@ -3518,20 +3518,20 @@
         <v>8</v>
       </c>
       <c r="E78" s="24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F78" s="25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G78" s="24" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H78" s="26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I78" s="24"/>
       <c r="J78" s="24" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K78" s="18">
         <v>29221887</v>
@@ -3544,29 +3544,29 @@
         <v>5</v>
       </c>
       <c r="B79" s="24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C79" s="24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D79" s="20" t="s">
         <v>8</v>
       </c>
       <c r="E79" s="24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F79" s="25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G79" s="24" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H79" s="26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I79" s="24"/>
       <c r="J79" s="24" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K79" s="18">
         <v>29221887</v>
@@ -3579,29 +3579,29 @@
         <v>5</v>
       </c>
       <c r="B80" s="24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C80" s="24" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D80" s="20" t="s">
         <v>8</v>
       </c>
       <c r="E80" s="24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F80" s="25" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G80" s="24" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H80" s="26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I80" s="24"/>
       <c r="J80" s="27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K80" s="18">
         <v>29221887</v>
@@ -3614,7 +3614,7 @@
         <v>5</v>
       </c>
       <c r="B81" s="24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C81" s="24" t="s">
         <v>7</v>
@@ -3623,20 +3623,20 @@
         <v>8</v>
       </c>
       <c r="E81" s="24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F81" s="25" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G81" s="24" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H81" s="26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I81" s="24"/>
       <c r="J81" s="24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K81" s="18">
         <v>29221887</v>
@@ -3649,7 +3649,7 @@
         <v>5</v>
       </c>
       <c r="B82" s="24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C82" s="24" t="s">
         <v>7</v>
@@ -3664,14 +3664,14 @@
         <v>6</v>
       </c>
       <c r="G82" s="24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H82" s="26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I82" s="24"/>
       <c r="J82" s="24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K82" s="19">
         <v>26575258</v>
@@ -3684,7 +3684,7 @@
         <v>5</v>
       </c>
       <c r="B83" s="24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C83" s="24" t="s">
         <v>7</v>
@@ -3699,14 +3699,14 @@
         <v>6</v>
       </c>
       <c r="G83" s="24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H83" s="26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I83" s="24"/>
       <c r="J83" s="24" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K83" s="19">
         <v>26575258</v>
@@ -3734,14 +3734,14 @@
         <v>6</v>
       </c>
       <c r="G84" s="24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H84" s="26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I84" s="24"/>
       <c r="J84" s="24" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K84" s="19">
         <v>26575258</v>
@@ -3754,10 +3754,10 @@
         <v>5</v>
       </c>
       <c r="B85" s="24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C85" s="24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D85" s="24" t="s">
         <v>8</v>
@@ -3769,14 +3769,14 @@
         <v>6</v>
       </c>
       <c r="G85" s="24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H85" s="26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I85" s="24"/>
       <c r="J85" s="24" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K85" s="19">
         <v>26575258</v>
@@ -3789,10 +3789,10 @@
         <v>5</v>
       </c>
       <c r="B86" s="24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C86" s="24" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D86" s="24" t="s">
         <v>8</v>
@@ -3804,14 +3804,14 @@
         <v>6</v>
       </c>
       <c r="G86" s="24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H86" s="26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I86" s="24"/>
       <c r="J86" s="27" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K86" s="19">
         <v>26575258</v>
@@ -3825,7 +3825,7 @@
         <v>1</v>
       </c>
       <c r="C87" s="24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D87" s="24" t="s">
         <v>8</v>
@@ -3837,14 +3837,14 @@
         <v>6</v>
       </c>
       <c r="G87" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H87" s="24" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I87" s="24"/>
       <c r="J87" s="25" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K87" s="19">
         <v>28564569</v>
@@ -3855,7 +3855,7 @@
     <row r="88" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A88" s="7"/>
       <c r="B88" s="24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C88" s="24" t="s">
         <v>7</v>
@@ -3870,14 +3870,14 @@
         <v>6</v>
       </c>
       <c r="G88" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H88" s="24" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I88" s="24"/>
       <c r="J88" s="25" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K88" s="19">
         <v>28564569</v>
@@ -3888,10 +3888,10 @@
     <row r="89" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A89" s="7"/>
       <c r="B89" s="24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C89" s="24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D89" s="24" t="s">
         <v>8</v>
@@ -3903,14 +3903,14 @@
         <v>6</v>
       </c>
       <c r="G89" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H89" s="24" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I89" s="24"/>
       <c r="J89" s="25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K89" s="19">
         <v>28564569</v>
@@ -3921,10 +3921,10 @@
     <row r="90" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A90" s="7"/>
       <c r="B90" s="24" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C90" s="24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D90" s="24" t="s">
         <v>8</v>
@@ -3936,14 +3936,14 @@
         <v>6</v>
       </c>
       <c r="G90" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H90" s="24" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I90" s="24"/>
       <c r="J90" s="25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K90" s="19">
         <v>28564569</v>
@@ -3954,10 +3954,10 @@
     <row r="91" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A91" s="7"/>
       <c r="B91" s="24" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C91" s="24" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D91" s="24" t="s">
         <v>8</v>
@@ -3969,14 +3969,14 @@
         <v>6</v>
       </c>
       <c r="G91" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H91" s="24" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I91" s="24"/>
       <c r="J91" s="28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K91" s="19">
         <v>28564569</v>
@@ -3990,7 +3990,7 @@
         <v>1</v>
       </c>
       <c r="C92" s="24" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D92" s="24" t="s">
         <v>8</v>
@@ -4002,14 +4002,14 @@
         <v>6</v>
       </c>
       <c r="G92" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H92" s="24" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I92" s="24"/>
       <c r="J92" s="25" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K92" s="19">
         <v>28564569</v>
@@ -4023,7 +4023,7 @@
         <v>1</v>
       </c>
       <c r="C93" s="24" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D93" s="24" t="s">
         <v>8</v>
@@ -4035,14 +4035,14 @@
         <v>6</v>
       </c>
       <c r="G93" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H93" s="24" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I93" s="24"/>
       <c r="J93" s="28" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K93" s="19">
         <v>28564569</v>
@@ -4068,14 +4068,14 @@
         <v>6</v>
       </c>
       <c r="G94" s="24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H94" s="24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I94" s="24"/>
       <c r="J94" s="25" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K94" s="19">
         <v>28564569</v>
@@ -4089,7 +4089,7 @@
         <v>1</v>
       </c>
       <c r="C95" s="24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D95" s="24" t="s">
         <v>8</v>
@@ -4101,14 +4101,14 @@
         <v>6</v>
       </c>
       <c r="G95" s="24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H95" s="24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I95" s="24"/>
       <c r="J95" s="25" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K95" s="19">
         <v>28564569</v>
@@ -4122,7 +4122,7 @@
         <v>1</v>
       </c>
       <c r="C96" s="24" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D96" s="24" t="s">
         <v>8</v>
@@ -4134,14 +4134,14 @@
         <v>6</v>
       </c>
       <c r="G96" s="24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H96" s="24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I96" s="24"/>
       <c r="J96" s="25" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K96" s="19">
         <v>28564569</v>
@@ -4155,7 +4155,7 @@
         <v>1</v>
       </c>
       <c r="C97" s="24" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D97" s="24" t="s">
         <v>8</v>
@@ -4167,14 +4167,14 @@
         <v>6</v>
       </c>
       <c r="G97" s="24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H97" s="24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I97" s="24"/>
       <c r="J97" s="25" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K97" s="19">
         <v>28564569</v>
@@ -4200,14 +4200,14 @@
         <v>6</v>
       </c>
       <c r="G98" s="24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H98" s="24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I98" s="24"/>
       <c r="J98" s="25" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K98" s="19">
         <v>28564569</v>
@@ -4218,7 +4218,7 @@
     <row r="99" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A99" s="7"/>
       <c r="B99" s="24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C99" s="24" t="s">
         <v>7</v>
@@ -4233,14 +4233,14 @@
         <v>6</v>
       </c>
       <c r="G99" s="24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H99" s="24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I99" s="24"/>
       <c r="J99" s="25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K99" s="19">
         <v>28564569</v>
@@ -4251,10 +4251,10 @@
     <row r="100" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A100" s="7"/>
       <c r="B100" s="24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C100" s="24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D100" s="24" t="s">
         <v>8</v>
@@ -4266,14 +4266,14 @@
         <v>6</v>
       </c>
       <c r="G100" s="24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H100" s="24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I100" s="24"/>
       <c r="J100" s="25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K100" s="19">
         <v>28564569</v>
@@ -4284,10 +4284,10 @@
     <row r="101" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A101" s="7"/>
       <c r="B101" s="24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C101" s="24" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D101" s="24" t="s">
         <v>8</v>
@@ -4299,14 +4299,14 @@
         <v>6</v>
       </c>
       <c r="G101" s="24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H101" s="24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I101" s="24"/>
       <c r="J101" s="28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K101" s="19">
         <v>28564569</v>
@@ -4317,10 +4317,10 @@
     <row r="102" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A102" s="7"/>
       <c r="B102" s="24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C102" s="24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D102" s="24" t="s">
         <v>8</v>
@@ -4332,14 +4332,14 @@
         <v>6</v>
       </c>
       <c r="G102" s="24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H102" s="24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I102" s="24"/>
       <c r="J102" s="25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K102" s="19">
         <v>28564569</v>
@@ -4350,10 +4350,10 @@
     <row r="103" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A103" s="7"/>
       <c r="B103" s="24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C103" s="24" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D103" s="24" t="s">
         <v>8</v>
@@ -4365,14 +4365,14 @@
         <v>6</v>
       </c>
       <c r="G103" s="24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H103" s="24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I103" s="24"/>
       <c r="J103" s="28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K103" s="19">
         <v>28564569</v>
@@ -4383,10 +4383,10 @@
     <row r="104" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A104" s="7"/>
       <c r="B104" s="24" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C104" s="24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D104" s="24" t="s">
         <v>8</v>
@@ -4398,14 +4398,14 @@
         <v>6</v>
       </c>
       <c r="G104" s="24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H104" s="24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I104" s="24"/>
       <c r="J104" s="25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K104" s="19">
         <v>28564569</v>
@@ -4416,10 +4416,10 @@
     <row r="105" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A105" s="7"/>
       <c r="B105" s="24" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C105" s="24" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D105" s="24" t="s">
         <v>8</v>
@@ -4431,14 +4431,14 @@
         <v>6</v>
       </c>
       <c r="G105" s="24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H105" s="24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I105" s="24"/>
       <c r="J105" s="28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K105" s="19">
         <v>28564569</v>
@@ -4449,10 +4449,10 @@
     <row r="106" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A106" s="7"/>
       <c r="B106" s="24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C106" s="24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D106" s="24" t="s">
         <v>8</v>
@@ -4464,14 +4464,14 @@
         <v>6</v>
       </c>
       <c r="G106" s="24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H106" s="24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I106" s="24"/>
       <c r="J106" s="25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K106" s="19">
         <v>28564569</v>
@@ -4482,10 +4482,10 @@
     <row r="107" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A107" s="7"/>
       <c r="B107" s="24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C107" s="24" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D107" s="24" t="s">
         <v>8</v>
@@ -4497,14 +4497,14 @@
         <v>6</v>
       </c>
       <c r="G107" s="24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H107" s="24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I107" s="24"/>
       <c r="J107" s="28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K107" s="19">
         <v>28564569</v>
@@ -4530,14 +4530,14 @@
         <v>6</v>
       </c>
       <c r="G108" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="H108" s="24" t="s">
         <v>134</v>
-      </c>
-      <c r="H108" s="24" t="s">
-        <v>135</v>
       </c>
       <c r="I108" s="24"/>
       <c r="J108" s="25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K108" s="18">
         <v>28498551</v>
@@ -4548,7 +4548,7 @@
     <row r="109" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A109" s="7"/>
       <c r="B109" s="24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C109" s="24" t="s">
         <v>7</v>
@@ -4563,14 +4563,14 @@
         <v>6</v>
       </c>
       <c r="G109" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="H109" s="24" t="s">
         <v>134</v>
-      </c>
-      <c r="H109" s="24" t="s">
-        <v>135</v>
       </c>
       <c r="I109" s="24"/>
       <c r="J109" s="25" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K109" s="18">
         <v>28498551</v>
@@ -4581,10 +4581,10 @@
     <row r="110" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A110" s="13"/>
       <c r="B110" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C110" s="24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D110" s="24" t="s">
         <v>8</v>
@@ -4596,14 +4596,14 @@
         <v>6</v>
       </c>
       <c r="G110" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="H110" s="24" t="s">
         <v>134</v>
-      </c>
-      <c r="H110" s="24" t="s">
-        <v>135</v>
       </c>
       <c r="I110" s="24"/>
       <c r="J110" s="25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K110" s="18">
         <v>28498551</v>
@@ -4614,7 +4614,7 @@
     <row r="111" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A111" s="13"/>
       <c r="B111" s="24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C111" s="24" t="s">
         <v>7</v>
@@ -4629,14 +4629,14 @@
         <v>6</v>
       </c>
       <c r="G111" s="24" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H111" s="24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I111" s="24"/>
       <c r="J111" s="25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K111" s="18">
         <v>26569658</v>
@@ -4647,7 +4647,7 @@
     <row r="112" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A112" s="13"/>
       <c r="B112" s="24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C112" s="24" t="s">
         <v>7</v>
@@ -4662,14 +4662,14 @@
         <v>6</v>
       </c>
       <c r="G112" s="24" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H112" s="24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I112" s="24"/>
       <c r="J112" s="25" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K112" s="18">
         <v>26569658</v>
@@ -4695,14 +4695,14 @@
         <v>6</v>
       </c>
       <c r="G113" s="24" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H113" s="24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I113" s="24"/>
       <c r="J113" s="25" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K113" s="18">
         <v>26569658</v>
@@ -4713,7 +4713,7 @@
     <row r="114" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A114" s="13"/>
       <c r="B114" s="24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C114" s="24" t="s">
         <v>7</v>
@@ -4728,14 +4728,14 @@
         <v>6</v>
       </c>
       <c r="G114" s="24" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H114" s="24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I114" s="24"/>
       <c r="J114" s="25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K114" s="18">
         <v>26569658</v>
@@ -4746,10 +4746,10 @@
     <row r="115" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A115" s="13"/>
       <c r="B115" s="24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C115" s="24" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D115" s="24" t="s">
         <v>8</v>
@@ -4761,14 +4761,14 @@
         <v>6</v>
       </c>
       <c r="G115" s="24" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H115" s="24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I115" s="24"/>
       <c r="J115" s="28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K115" s="18">
         <v>26569658</v>
@@ -4779,10 +4779,10 @@
     <row r="116" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A116" s="13"/>
       <c r="B116" s="24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C116" s="24" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D116" s="24" t="s">
         <v>8</v>
@@ -4794,14 +4794,14 @@
         <v>6</v>
       </c>
       <c r="G116" s="24" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H116" s="24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I116" s="24"/>
       <c r="J116" s="28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K116" s="18">
         <v>26569658</v>
@@ -4815,7 +4815,7 @@
         <v>1</v>
       </c>
       <c r="C117" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D117" s="24" t="s">
         <v>8</v>
@@ -4827,14 +4827,14 @@
         <v>6</v>
       </c>
       <c r="G117" s="24" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H117" s="24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I117" s="24"/>
       <c r="J117" s="25" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K117" s="18">
         <v>26569658</v>
@@ -4845,10 +4845,10 @@
     <row r="118" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A118" s="13"/>
       <c r="B118" s="24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C118" s="24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D118" s="24" t="s">
         <v>8</v>
@@ -4860,14 +4860,14 @@
         <v>6</v>
       </c>
       <c r="G118" s="24" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H118" s="24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I118" s="24"/>
       <c r="J118" s="25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K118" s="18">
         <v>26569658</v>
@@ -4878,10 +4878,10 @@
     <row r="119" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A119" s="13"/>
       <c r="B119" s="24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C119" s="24" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D119" s="24" t="s">
         <v>8</v>
@@ -4893,14 +4893,14 @@
         <v>6</v>
       </c>
       <c r="G119" s="24" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H119" s="24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I119" s="24"/>
       <c r="J119" s="28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K119" s="18">
         <v>26569658</v>
@@ -4914,7 +4914,7 @@
         <v>1</v>
       </c>
       <c r="C120" s="24" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D120" s="24" t="s">
         <v>8</v>
@@ -4926,14 +4926,14 @@
         <v>6</v>
       </c>
       <c r="G120" s="24" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H120" s="24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I120" s="24"/>
       <c r="J120" s="25" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K120" s="18">
         <v>26569658</v>
@@ -4947,7 +4947,7 @@
         <v>1</v>
       </c>
       <c r="C121" s="24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D121" s="24" t="s">
         <v>8</v>
@@ -4959,14 +4959,14 @@
         <v>6</v>
       </c>
       <c r="G121" s="24" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H121" s="24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I121" s="24"/>
       <c r="J121" s="25" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K121" s="18">
         <v>26569658</v>
@@ -4977,10 +4977,10 @@
     <row r="122" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A122" s="7"/>
       <c r="B122" s="24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C122" s="24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D122" s="24" t="s">
         <v>8</v>
@@ -4989,7 +4989,7 @@
         <v>2</v>
       </c>
       <c r="F122" s="25" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G122" s="24"/>
       <c r="H122" s="24"/>
@@ -5004,10 +5004,10 @@
     <row r="123" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A123" s="7"/>
       <c r="B123" s="24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C123" s="24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D123" s="24" t="s">
         <v>8</v>
@@ -5016,7 +5016,7 @@
         <v>2</v>
       </c>
       <c r="F123" s="25" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G123" s="24"/>
       <c r="H123" s="26"/>
@@ -5055,7 +5055,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A7"/>
     </sheetView>
   </sheetViews>
@@ -5066,47 +5066,47 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>